<commit_message>
Add best exam and worst exam for evaluating multiple bugs
</commit_message>
<xml_diff>
--- a/experiment_results/SBFL_ONLY/Summary/Elevator/multiple_bugs_123bug.xlsx
+++ b/experiment_results/SBFL_ONLY/Summary/Elevator/multiple_bugs_123bug.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="9">
   <si>
     <t>EVALUATION_METRIC</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Worst rank</t>
+  </si>
+  <si>
+    <t>Best exam</t>
+  </si>
+  <si>
+    <t>Worst exam</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -514,6 +520,22 @@
         <v>111.672131147541</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>2.162617096018736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>24.9268149882904</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -521,7 +543,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -640,6 +662,22 @@
         <v>101.8770491803279</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.90463992974239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>22.74041276346604</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -647,7 +685,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -766,6 +804,22 @@
         <v>191.2868852459016</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.90281030444965</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>42.69796545667447</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -773,7 +827,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -892,6 +946,22 @@
         <v>296.9672131147541</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>12.12492681498831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>66.28732435597188</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -899,7 +969,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1018,6 +1088,22 @@
         <v>296.9672131147541</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>12.12492681498831</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>66.28732435597188</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1025,7 +1111,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1144,6 +1230,22 @@
         <v>186.6475409836065</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.295374707259954</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>41.66239754098361</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1151,7 +1253,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1270,6 +1372,22 @@
         <v>108.4262295081967</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.063012295081968</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>24.20228337236534</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1277,7 +1395,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1396,6 +1514,22 @@
         <v>125.0819672131148</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>5.122950819672131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>27.92008196721311</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1403,7 +1537,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1522,6 +1656,22 @@
         <v>340.4098360655738</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>26.88085480093671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>75.98433840749414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1529,7 +1679,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1648,6 +1798,22 @@
         <v>101.8770491803279</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.90463992974239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>22.74041276346604</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1655,7 +1821,7 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1774,6 +1940,22 @@
         <v>101.8770491803279</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.90463992974239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>22.74041276346604</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1781,7 +1963,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1900,6 +2082,22 @@
         <v>103.1475409836066</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.216700819672132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>23.02400468384074</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1907,7 +2105,7 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2026,6 +2224,22 @@
         <v>340.4098360655738</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>26.88085480093671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>75.98433840749414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2033,7 +2247,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2152,6 +2366,22 @@
         <v>340.4098360655738</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>26.88085480093671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>75.98433840749414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2159,7 +2389,7 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2278,6 +2508,22 @@
         <v>340.4098360655738</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>26.88085480093671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>75.98433840749414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2285,7 +2531,7 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2404,6 +2650,22 @@
         <v>105.9344262295082</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>2.083943208430914</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>23.64607728337236</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2411,7 +2673,7 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2530,6 +2792,22 @@
         <v>180.4098360655738</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>0.9989754098360663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>40.27005269320841</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2537,7 +2815,7 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2656,6 +2934,22 @@
         <v>340.4098360655738</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>26.88085480093671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>75.98433840749414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2663,7 +2957,7 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2782,6 +3076,22 @@
         <v>298.5409836065574</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>11.84865339578455</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>66.63861241217795</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2789,7 +3099,7 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2908,6 +3218,22 @@
         <v>101.8770491803279</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.90463992974239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>22.74041276346604</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2915,7 +3241,7 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3034,6 +3360,22 @@
         <v>101.8770491803279</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.90463992974239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>22.74041276346604</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3041,7 +3383,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3160,6 +3502,22 @@
         <v>186.0573770491803</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>0.9989754098360663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>41.53066451990631</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3167,7 +3525,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3286,6 +3644,22 @@
         <v>109.5081967213115</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>3.128659250585479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>24.44379391100702</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3293,7 +3667,7 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3412,6 +3786,22 @@
         <v>111.3934426229508</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.51492974238876</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>24.86460772833722</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3419,7 +3809,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3538,6 +3928,22 @@
         <v>111.672131147541</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>2.162617096018736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>24.9268149882904</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3545,7 +3951,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3664,6 +4070,22 @@
         <v>103.3770491803279</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.200234192037472</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>23.07523419203747</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3671,7 +4093,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3790,6 +4212,22 @@
         <v>125.0819672131148</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>5.122950819672131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>27.92008196721311</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3797,7 +4235,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3916,6 +4354,22 @@
         <v>340.4098360655738</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>26.88085480093671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>75.98433840749414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3923,7 +4377,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4042,6 +4496,22 @@
         <v>340.4098360655738</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>26.88085480093671</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>75.98433840749414</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4049,7 +4519,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4168,6 +4638,22 @@
         <v>128.5655737704918</v>
       </c>
     </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1.004464285714287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>28.69767271662765</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>